<commit_message>
corrections and finish of 1.5
</commit_message>
<xml_diff>
--- a/A2_results_step1.5_oneprice.xlsx
+++ b/A2_results_step1.5_oneprice.xlsx
@@ -27,9 +27,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>x1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>x4</t>
+  </si>
+  <si>
+    <t>x5</t>
+  </si>
+  <si>
+    <t>x6</t>
+  </si>
+  <si>
+    <t>x7</t>
+  </si>
+  <si>
+    <t>x8</t>
+  </si>
+  <si>
+    <t>x9</t>
+  </si>
+  <si>
+    <t>x10</t>
+  </si>
+  <si>
+    <t>x11</t>
+  </si>
+  <si>
+    <t>x12</t>
+  </si>
+  <si>
+    <t>x13</t>
+  </si>
+  <si>
+    <t>x14</t>
+  </si>
+  <si>
+    <t>x15</t>
+  </si>
+  <si>
+    <t>x16</t>
+  </si>
+  <si>
+    <t>x17</t>
+  </si>
+  <si>
+    <t>x18</t>
+  </si>
+  <si>
+    <t>x19</t>
+  </si>
+  <si>
+    <t>x20</t>
+  </si>
+  <si>
+    <t>x21</t>
+  </si>
+  <si>
+    <t>x22</t>
+  </si>
+  <si>
+    <t>x23</t>
+  </si>
+  <si>
+    <t>x24</t>
   </si>
 </sst>
 </file>
@@ -2399,134 +2468,157 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2">
         <v>71865.48750000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
+      <c r="B2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
+      <c r="C2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5">
+      <c r="D2">
         <v>66867.11249999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6">
+      <c r="E2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7">
+      <c r="F2">
         <v>85071.02999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8">
+      <c r="G2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9">
+      <c r="H2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10">
+      <c r="I2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11">
+      <c r="J2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12">
+      <c r="K2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13">
+      <c r="L2">
         <v>76175.91</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14">
+      <c r="M2">
         <v>71629.39499999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15">
+      <c r="N2">
         <v>69435.38250000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16">
+      <c r="O2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17">
+      <c r="P2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18">
+      <c r="Q2">
         <v>89052.57</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19">
+      <c r="R2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20">
+      <c r="S2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21">
+      <c r="T2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22">
+      <c r="U2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23">
+      <c r="V2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24">
+      <c r="W2">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25">
+      <c r="X2">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>